<commit_message>
passwed with some changes and fixes
</commit_message>
<xml_diff>
--- a/SecondTask/Statistics.xlsx
+++ b/SecondTask/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\ThirdCourse\PP\SecondTask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBB70D7-C7CE-45ED-9580-DE5C68630D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55361D6D-F926-41C4-86CC-E7C97A042A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
   <si>
     <t>1-ядерный</t>
   </si>
@@ -63,33 +63,6 @@
   </si>
   <si>
     <t>Эффективность ускорения</t>
-  </si>
-  <si>
-    <t>Вывод</t>
-  </si>
-  <si>
-    <t>На 2,3,4 ядрах видна линейная зависимость со 2 потока. На 1 ядре время выполнения не подчинается ни линейной, ни нелинейной зависимости</t>
-  </si>
-  <si>
-    <t>При работе на одном ядре время выполнения колеблится в пределах 3,62 секунд, начиная со 2 потока на 2,3,4 ядрах время выполнения стремится к 3, 1.9, 1.6 секунд соотвественно</t>
-  </si>
-  <si>
-    <t>Выводы</t>
-  </si>
-  <si>
-    <t>Ускорение при работе с одним ядром колебится в пределах 1,005 (Незначительный прирост)</t>
-  </si>
-  <si>
-    <t>При работе с двумя ядрами ускорение колебится в районе 1.2 после скачка с 1</t>
-  </si>
-  <si>
-    <t>Эффективность ускорения имеет экспоненциальный вид на 1-4 ядрах, прирост эффективности колеблется на уровне сотых разрядов</t>
-  </si>
-  <si>
-    <t>Аналогично двум ядрам, наблюдается резкий скачок для 3 ядер на 2 и на 2.1 для 4</t>
-  </si>
-  <si>
-    <t>При работе с 2,3,4 ядрами устанавливается линейная зависимость, начиная со 2-4 потоков. (Приблизительно в 2 раза больше)</t>
   </si>
 </sst>
 </file>
@@ -186,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -195,27 +168,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -11550,10 +11516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD139"/>
+  <dimension ref="A1:AD96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11724,9 +11690,6 @@
       <c r="K6" s="1">
         <v>1.702</v>
       </c>
-      <c r="M6" s="12" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -11753,26 +11716,24 @@
       <c r="K7" s="1">
         <v>1.7070000000000001</v>
       </c>
-      <c r="M7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="14"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -11799,24 +11760,24 @@
       <c r="K8" s="1">
         <v>1.7030000000000001</v>
       </c>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="14"/>
-      <c r="AD8" s="14"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -11843,23 +11804,21 @@
       <c r="K9" s="1">
         <v>1.704</v>
       </c>
-      <c r="M9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -11886,21 +11845,21 @@
       <c r="K10" s="5">
         <v>1.7170000000000001</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="8"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -11927,23 +11886,21 @@
       <c r="K11" s="1">
         <v>1.708</v>
       </c>
-      <c r="M11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
-      <c r="AA11" s="8"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
@@ -11970,21 +11927,21 @@
       <c r="K12" s="1">
         <v>1.7130000000000001</v>
       </c>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="8"/>
-      <c r="AA12" s="8"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
@@ -12130,12 +12087,12 @@
       <c r="A20" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
+      <c r="A38" s="8"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
@@ -12158,19 +12115,19 @@
       <c r="A40" s="2">
         <v>1</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="6">
         <f>$B$2/$B2</f>
         <v>1</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="6">
         <f>$E$2/$E2</f>
         <v>1</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="6">
         <f>$H$2/$H2</f>
         <v>1</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="6">
         <f>$K$2/$K2</f>
         <v>1</v>
       </c>
@@ -12179,19 +12136,19 @@
       <c r="A41" s="2">
         <v>2</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="6">
         <f t="shared" ref="B41:B55" si="0">$B$2/$B3</f>
         <v>1.0091488771832549</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="6">
         <f t="shared" ref="C41:C55" si="1">$E$2/$E3</f>
         <v>1.1955288621955289</v>
       </c>
-      <c r="D41" s="10">
-        <f t="shared" ref="D41:D55" si="2">$H$2/$H3</f>
+      <c r="D41" s="6">
+        <f t="shared" ref="D41:D54" si="2">$H$2/$H3</f>
         <v>1.8696985181400101</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="6">
         <f t="shared" ref="E41:E55" si="3">$K$2/$K3</f>
         <v>1.5085168259243871</v>
       </c>
@@ -12200,19 +12157,19 @@
       <c r="A42" s="2">
         <v>3</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="6">
         <f t="shared" si="0"/>
         <v>1.0027548209366393</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="6">
         <f t="shared" si="1"/>
         <v>1.1967267869071476</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="6">
         <f t="shared" si="2"/>
         <v>2.007131102578168</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="6">
         <f t="shared" si="3"/>
         <v>1.7609117361784676</v>
       </c>
@@ -12221,19 +12178,19 @@
       <c r="A43" s="2">
         <v>4</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="6">
         <f t="shared" si="0"/>
         <v>1.0125173852573017</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="6">
         <f t="shared" si="1"/>
         <v>1.2011397921555482</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="6">
         <f t="shared" si="2"/>
         <v>1.9370037056643725</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="6">
         <f t="shared" si="3"/>
         <v>2.1012731481481479</v>
       </c>
@@ -12242,19 +12199,19 @@
       <c r="A44" s="2">
         <v>5</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="6">
         <f t="shared" si="0"/>
         <v>1.0019267822736031</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="6">
         <f t="shared" si="1"/>
         <v>1.1999330207635632</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="6">
         <f t="shared" si="2"/>
         <v>1.9918345127925965</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="6">
         <f t="shared" si="3"/>
         <v>2.1333725029377204</v>
       </c>
@@ -12263,19 +12220,19 @@
       <c r="A45" s="2">
         <v>6</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="6">
         <f t="shared" si="0"/>
         <v>1.0105496946141033</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="6">
         <f t="shared" si="1"/>
         <v>1.19953130231001</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="6">
         <f t="shared" si="2"/>
         <v>1.9842733188720172</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="6">
         <f t="shared" si="3"/>
         <v>2.1271236086701815</v>
       </c>
@@ -12284,19 +12241,19 @@
       <c r="A46" s="2">
         <v>7</v>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="6">
         <f t="shared" si="0"/>
         <v>1.0083102493074794</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="6">
         <f t="shared" si="1"/>
         <v>1.1999330207635632</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="6">
         <f t="shared" si="2"/>
         <v>2.0093355299286104</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="6">
         <f t="shared" si="3"/>
         <v>2.1321197886083381</v>
       </c>
@@ -12305,19 +12262,19 @@
       <c r="A47" s="2">
         <v>8</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="6">
         <f t="shared" si="0"/>
         <v>1.0055248618784531</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="6">
         <f t="shared" si="1"/>
         <v>1.1979271146773653</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="6">
         <f t="shared" si="2"/>
         <v>1.9940054495912807</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47" s="6">
         <f t="shared" si="3"/>
         <v>2.130868544600939</v>
       </c>
@@ -12326,224 +12283,205 @@
       <c r="A48" s="2">
         <v>9</v>
       </c>
-      <c r="B48" s="10">
+      <c r="B48" s="6">
         <f t="shared" si="0"/>
         <v>1.006358860934476</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="6">
         <f t="shared" si="1"/>
         <v>1.1991298527443106</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="6">
         <f t="shared" si="2"/>
         <v>2.0104395604395604</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="6">
         <f t="shared" si="3"/>
         <v>2.1147350029120555</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>10</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B49" s="6">
         <f t="shared" si="0"/>
         <v>0.99862825788751719</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="6">
         <f t="shared" si="1"/>
         <v>1.1987286717965877</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D49" s="6">
         <f t="shared" si="2"/>
         <v>2.0282705099778271</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49" s="6">
         <f t="shared" si="3"/>
         <v>2.1258782201405153</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>11</v>
       </c>
-      <c r="B50" s="10">
+      <c r="B50" s="6">
         <f t="shared" si="0"/>
         <v>1.0013755158184321</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="6">
         <f t="shared" si="1"/>
         <v>1.1987286717965877</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="6">
         <f t="shared" si="2"/>
         <v>2.0249031543995573</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="6">
         <f t="shared" si="3"/>
         <v>2.1196730881494452</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>12</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="6">
         <f t="shared" si="0"/>
         <v>1.0052471692902514</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="6">
         <f t="shared" si="1"/>
         <v>1.2003350083752096</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D51" s="6">
         <f t="shared" si="2"/>
         <v>2.027146814404432</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E51" s="6">
         <f t="shared" si="3"/>
         <v>2.1147350029120555</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>13</v>
       </c>
-      <c r="B52" s="10">
+      <c r="B52" s="6">
         <f t="shared" si="0"/>
         <v>1.0035842293906811</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="6">
         <f t="shared" si="1"/>
         <v>1.19953130231001</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="6">
         <f t="shared" si="2"/>
         <v>2.0226644555002764</v>
       </c>
-      <c r="E52" s="10">
+      <c r="E52" s="6">
         <f t="shared" si="3"/>
         <v>2.1159673659673657</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>14</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="6">
         <f t="shared" si="0"/>
         <v>1.0033076074972436</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C53" s="6">
         <f t="shared" si="1"/>
         <v>1.1971266288005347</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D53" s="6">
         <f t="shared" si="2"/>
         <v>2.0260243632336654</v>
       </c>
-      <c r="E53" s="10">
+      <c r="E53" s="6">
         <f t="shared" si="3"/>
         <v>2.1196730881494452</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>15</v>
       </c>
-      <c r="B54" s="10">
+      <c r="B54" s="6">
         <f t="shared" si="0"/>
         <v>1.0102692200943657</v>
       </c>
-      <c r="C54" s="10">
+      <c r="C54" s="6">
         <f t="shared" si="1"/>
         <v>1.2007372654155497</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D54" s="6">
         <f t="shared" si="2"/>
         <v>2.0305216426193118</v>
       </c>
-      <c r="E54" s="10">
+      <c r="E54" s="6">
         <f t="shared" si="3"/>
         <v>2.1135040745052387</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>16</v>
       </c>
-      <c r="B55" s="10">
+      <c r="B55" s="6">
         <f t="shared" si="0"/>
         <v>1.006080707573245</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="6">
         <f t="shared" si="1"/>
         <v>1.19953130231001</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D55" s="6">
         <f>$H$2/$H17</f>
         <v>2.0159779614325068</v>
       </c>
-      <c r="E55" s="10">
+      <c r="E55" s="6">
         <f t="shared" si="3"/>
         <v>2.1196730881494452</v>
       </c>
-      <c r="H55" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="H56" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="8"/>
-      <c r="O56" s="8"/>
-      <c r="P56" s="13"/>
-      <c r="Q56" s="13"/>
-      <c r="R56" s="13"/>
-      <c r="S56" s="13"/>
-      <c r="T56" s="13"/>
-      <c r="U56" s="13"/>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
+      <c r="N56" s="10"/>
+      <c r="O56" s="10"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A57" s="11" t="s">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
-      <c r="M57" s="8"/>
-      <c r="N57" s="8"/>
-      <c r="O57" s="8"/>
-      <c r="P57" s="13"/>
-      <c r="Q57" s="13"/>
-      <c r="R57" s="13"/>
-      <c r="S57" s="13"/>
-      <c r="T57" s="13"/>
-      <c r="U57" s="13"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10"/>
+      <c r="O57" s="10"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A58" s="11"/>
-      <c r="H58" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="8"/>
-      <c r="M58" s="8"/>
-      <c r="N58" s="8"/>
-      <c r="O58" s="8"/>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
+      <c r="N58" s="10"/>
+      <c r="O58" s="10"/>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>2</v>
       </c>
@@ -12559,134 +12497,132 @@
       <c r="E59" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="8"/>
-      <c r="M59" s="8"/>
-      <c r="N59" s="8"/>
-      <c r="O59" s="8"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="10"/>
+      <c r="N59" s="10"/>
+      <c r="O59" s="10"/>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>1</v>
       </c>
-      <c r="B60" s="10">
+      <c r="B60" s="6">
         <f>B40/$A60</f>
         <v>1</v>
       </c>
-      <c r="C60" s="10">
+      <c r="C60" s="6">
         <f t="shared" ref="C60:E60" si="4">C40/$A60</f>
         <v>1</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D60" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E60" s="10">
+      <c r="E60" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="H60" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
-      <c r="L60" s="6"/>
-      <c r="M60" s="6"/>
-      <c r="N60" s="6"/>
-      <c r="O60" s="6"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>2</v>
       </c>
-      <c r="B61" s="10">
+      <c r="B61" s="6">
         <f t="shared" ref="B61:E75" si="5">B41/$A61</f>
         <v>0.50457443859162743</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C61" s="6">
         <f t="shared" si="5"/>
         <v>0.59776443109776445</v>
       </c>
-      <c r="D61" s="10">
+      <c r="D61" s="6">
         <f t="shared" si="5"/>
         <v>0.93484925907000505</v>
       </c>
-      <c r="E61" s="10">
+      <c r="E61" s="6">
         <f t="shared" si="5"/>
         <v>0.75425841296219354</v>
       </c>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="M61" s="6"/>
-      <c r="N61" s="6"/>
-      <c r="O61" s="6"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="11"/>
+      <c r="O61" s="11"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>3</v>
       </c>
-      <c r="B62" s="10">
+      <c r="B62" s="6">
         <f t="shared" si="5"/>
         <v>0.33425160697887973</v>
       </c>
-      <c r="C62" s="10">
+      <c r="C62" s="6">
         <f t="shared" si="5"/>
         <v>0.39890892896904923</v>
       </c>
-      <c r="D62" s="10">
+      <c r="D62" s="6">
         <f t="shared" si="5"/>
         <v>0.66904370085938936</v>
       </c>
-      <c r="E62" s="10">
+      <c r="E62" s="6">
         <f t="shared" si="5"/>
         <v>0.58697057872615588</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>4</v>
       </c>
-      <c r="B63" s="10">
+      <c r="B63" s="6">
         <f t="shared" si="5"/>
         <v>0.25312934631432543</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="6">
         <f t="shared" si="5"/>
         <v>0.30028494803888706</v>
       </c>
-      <c r="D63" s="10">
+      <c r="D63" s="6">
         <f t="shared" si="5"/>
         <v>0.48425092641609313</v>
       </c>
-      <c r="E63" s="10">
+      <c r="E63" s="6">
         <f t="shared" si="5"/>
         <v>0.52531828703703698</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>5</v>
       </c>
-      <c r="B64" s="10">
+      <c r="B64" s="6">
         <f t="shared" si="5"/>
         <v>0.20038535645472061</v>
       </c>
-      <c r="C64" s="10">
+      <c r="C64" s="6">
         <f t="shared" si="5"/>
         <v>0.23998660415271264</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D64" s="6">
         <f t="shared" si="5"/>
         <v>0.39836690255851931</v>
       </c>
-      <c r="E64" s="10">
+      <c r="E64" s="6">
         <f t="shared" si="5"/>
         <v>0.42667450058754408</v>
       </c>
@@ -12695,19 +12631,19 @@
       <c r="A65" s="2">
         <v>6</v>
       </c>
-      <c r="B65" s="10">
+      <c r="B65" s="6">
         <f t="shared" si="5"/>
         <v>0.16842494910235054</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="6">
         <f t="shared" si="5"/>
         <v>0.199921883718335</v>
       </c>
-      <c r="D65" s="10">
+      <c r="D65" s="6">
         <f t="shared" si="5"/>
         <v>0.33071221981200288</v>
       </c>
-      <c r="E65" s="10">
+      <c r="E65" s="6">
         <f t="shared" si="5"/>
         <v>0.35452060144503023</v>
       </c>
@@ -12716,19 +12652,19 @@
       <c r="A66" s="2">
         <v>7</v>
       </c>
-      <c r="B66" s="10">
+      <c r="B66" s="6">
         <f t="shared" si="5"/>
         <v>0.1440443213296399</v>
       </c>
-      <c r="C66" s="10">
+      <c r="C66" s="6">
         <f t="shared" si="5"/>
         <v>0.17141900296622331</v>
       </c>
-      <c r="D66" s="10">
+      <c r="D66" s="6">
         <f t="shared" si="5"/>
         <v>0.28704793284694435</v>
       </c>
-      <c r="E66" s="10">
+      <c r="E66" s="6">
         <f t="shared" si="5"/>
         <v>0.30458854122976259</v>
       </c>
@@ -12737,19 +12673,19 @@
       <c r="A67" s="2">
         <v>8</v>
       </c>
-      <c r="B67" s="10">
+      <c r="B67" s="6">
         <f t="shared" si="5"/>
         <v>0.12569060773480664</v>
       </c>
-      <c r="C67" s="10">
+      <c r="C67" s="6">
         <f t="shared" si="5"/>
         <v>0.14974088933467067</v>
       </c>
-      <c r="D67" s="10">
+      <c r="D67" s="6">
         <f t="shared" si="5"/>
         <v>0.24925068119891008</v>
       </c>
-      <c r="E67" s="10">
+      <c r="E67" s="6">
         <f t="shared" si="5"/>
         <v>0.26635856807511737</v>
       </c>
@@ -12758,19 +12694,19 @@
       <c r="A68" s="2">
         <v>9</v>
       </c>
-      <c r="B68" s="10">
+      <c r="B68" s="6">
         <f t="shared" si="5"/>
         <v>0.11181765121494178</v>
       </c>
-      <c r="C68" s="10">
+      <c r="C68" s="6">
         <f t="shared" si="5"/>
         <v>0.1332366503049234</v>
       </c>
-      <c r="D68" s="10">
+      <c r="D68" s="6">
         <f t="shared" si="5"/>
         <v>0.22338217338217337</v>
       </c>
-      <c r="E68" s="10">
+      <c r="E68" s="6">
         <f t="shared" si="5"/>
         <v>0.23497055587911728</v>
       </c>
@@ -12779,19 +12715,19 @@
       <c r="A69" s="2">
         <v>10</v>
       </c>
-      <c r="B69" s="10">
+      <c r="B69" s="6">
         <f t="shared" si="5"/>
         <v>9.9862825788751719E-2</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="6">
         <f t="shared" si="5"/>
         <v>0.11987286717965877</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D69" s="6">
         <f t="shared" si="5"/>
         <v>0.2028270509977827</v>
       </c>
-      <c r="E69" s="10">
+      <c r="E69" s="6">
         <f t="shared" si="5"/>
         <v>0.21258782201405152</v>
       </c>
@@ -12800,19 +12736,19 @@
       <c r="A70" s="2">
         <v>11</v>
       </c>
-      <c r="B70" s="10">
+      <c r="B70" s="6">
         <f t="shared" si="5"/>
         <v>9.1034137801675644E-2</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C70" s="6">
         <f t="shared" si="5"/>
         <v>0.10897533379968979</v>
       </c>
-      <c r="D70" s="10">
+      <c r="D70" s="6">
         <f t="shared" si="5"/>
         <v>0.1840821049454143</v>
       </c>
-      <c r="E70" s="10">
+      <c r="E70" s="6">
         <f t="shared" si="5"/>
         <v>0.19269755346813139</v>
       </c>
@@ -12821,19 +12757,19 @@
       <c r="A71" s="2">
         <v>12</v>
       </c>
-      <c r="B71" s="10">
+      <c r="B71" s="6">
         <f t="shared" si="5"/>
         <v>8.3770597440854286E-2</v>
       </c>
-      <c r="C71" s="10">
+      <c r="C71" s="6">
         <f t="shared" si="5"/>
         <v>0.1000279173646008</v>
       </c>
-      <c r="D71" s="10">
+      <c r="D71" s="6">
         <f t="shared" si="5"/>
         <v>0.16892890120036932</v>
       </c>
-      <c r="E71" s="10">
+      <c r="E71" s="6">
         <f t="shared" si="5"/>
         <v>0.17622791690933795</v>
       </c>
@@ -12842,19 +12778,19 @@
       <c r="A72" s="2">
         <v>13</v>
       </c>
-      <c r="B72" s="10">
+      <c r="B72" s="6">
         <f t="shared" si="5"/>
         <v>7.7198786876206238E-2</v>
       </c>
-      <c r="C72" s="10">
+      <c r="C72" s="6">
         <f t="shared" si="5"/>
         <v>9.2271638639231546E-2</v>
       </c>
-      <c r="D72" s="10">
+      <c r="D72" s="6">
         <f t="shared" si="5"/>
         <v>0.15558957350002126</v>
       </c>
-      <c r="E72" s="10">
+      <c r="E72" s="6">
         <f t="shared" si="5"/>
         <v>0.16276672045902812</v>
       </c>
@@ -12863,19 +12799,19 @@
       <c r="A73" s="2">
         <v>14</v>
       </c>
-      <c r="B73" s="10">
+      <c r="B73" s="6">
         <f t="shared" si="5"/>
         <v>7.1664829106945965E-2</v>
       </c>
-      <c r="C73" s="10">
+      <c r="C73" s="6">
         <f t="shared" si="5"/>
         <v>8.5509044914323901E-2</v>
       </c>
-      <c r="D73" s="10">
+      <c r="D73" s="6">
         <f t="shared" si="5"/>
         <v>0.14471602594526181</v>
       </c>
-      <c r="E73" s="10">
+      <c r="E73" s="6">
         <f t="shared" si="5"/>
         <v>0.15140522058210323</v>
       </c>
@@ -12884,19 +12820,19 @@
       <c r="A74" s="2">
         <v>15</v>
       </c>
-      <c r="B74" s="10">
+      <c r="B74" s="6">
         <f t="shared" si="5"/>
         <v>6.7351281339624383E-2</v>
       </c>
-      <c r="C74" s="10">
+      <c r="C74" s="6">
         <f t="shared" si="5"/>
         <v>8.0049151027703311E-2</v>
       </c>
-      <c r="D74" s="10">
+      <c r="D74" s="6">
         <f t="shared" si="5"/>
         <v>0.13536810950795411</v>
       </c>
-      <c r="E74" s="10">
+      <c r="E74" s="6">
         <f t="shared" si="5"/>
         <v>0.14090027163368257</v>
       </c>
@@ -12905,80 +12841,50 @@
       <c r="A75" s="2">
         <v>16</v>
       </c>
-      <c r="B75" s="10">
+      <c r="B75" s="6">
         <f t="shared" si="5"/>
         <v>6.2880044223327811E-2</v>
       </c>
-      <c r="C75" s="10">
+      <c r="C75" s="6">
         <f t="shared" si="5"/>
         <v>7.4970706394375627E-2</v>
       </c>
-      <c r="D75" s="10">
+      <c r="D75" s="6">
         <f t="shared" si="5"/>
         <v>0.12599862258953168</v>
       </c>
-      <c r="E75" s="10">
+      <c r="E75" s="6">
         <f t="shared" si="5"/>
         <v>0.13247956800934033</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B95" s="14"/>
-      <c r="C95" s="14"/>
-      <c r="D95" s="14"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="14"/>
-      <c r="H95" s="14"/>
-      <c r="I95" s="14"/>
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="14"/>
-      <c r="B96" s="14"/>
-      <c r="C96" s="14"/>
-      <c r="D96" s="14"/>
-      <c r="E96" s="14"/>
-      <c r="F96" s="14"/>
-      <c r="G96" s="14"/>
-      <c r="H96" s="14"/>
-      <c r="I96" s="14"/>
-    </row>
-    <row r="138" spans="10:15" x14ac:dyDescent="0.3">
-      <c r="J138" s="13"/>
-      <c r="K138" s="13"/>
-      <c r="L138" s="13"/>
-      <c r="M138" s="13"/>
-      <c r="N138" s="13"/>
-      <c r="O138" s="13"/>
-    </row>
-    <row r="139" spans="10:15" x14ac:dyDescent="0.3">
-      <c r="J139" s="13"/>
-      <c r="K139" s="13"/>
-      <c r="L139" s="13"/>
-      <c r="M139" s="13"/>
-      <c r="N139" s="13"/>
-      <c r="O139" s="13"/>
+      <c r="A96" s="10"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="10"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="M9:AA10"/>
-    <mergeCell ref="H56:O57"/>
-    <mergeCell ref="H58:O59"/>
-    <mergeCell ref="H60:O61"/>
-    <mergeCell ref="A95:I96"/>
+  <mergeCells count="3">
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="A57:A58"/>
-    <mergeCell ref="M11:AA12"/>
-    <mergeCell ref="M7:AD8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>